<commit_message>
adjust page of new_web
</commit_message>
<xml_diff>
--- a/data/The history of global natural gas production.xlsx
+++ b/data/The history of global natural gas production.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSS5201_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06671E38-D895-4ED4-8715-FCA84E61EE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD8057F-A7F6-4F0A-AEED-AA192190A6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15510,8 +15510,8 @@
   </sheetPr>
   <dimension ref="A1:B221"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A212" sqref="A212"/>
+    <sheetView topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17297,11 +17297,14 @@
   </sheetPr>
   <dimension ref="A1:CY124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="BL37" sqref="BL37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -49443,17 +49446,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="CS52:CT52"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="BX63:BY63"/>
-    <mergeCell ref="BI60:BJ60"/>
-    <mergeCell ref="BI69:BJ69"/>
     <mergeCell ref="Q76:R76"/>
     <mergeCell ref="Q77:R77"/>
     <mergeCell ref="Q49:R49"/>
     <mergeCell ref="Q50:R50"/>
     <mergeCell ref="Q51:R51"/>
     <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="CS52:CT52"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="BX63:BY63"/>
+    <mergeCell ref="BI60:BJ60"/>
+    <mergeCell ref="BI69:BJ69"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>